<commit_message>
doc: 2020-01-15 공부한 것 추가
</commit_message>
<xml_diff>
--- a/documents/20200114/회원관리URL매핑정책.xlsx
+++ b/documents/20200114/회원관리URL매핑정책.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21000" windowHeight="13740"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21000" windowHeight="13740" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="66">
   <si>
     <t>기능</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -157,123 +157,127 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>로그인처리</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>id,pw</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>화면이동</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>회원수정</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>회원수정처리</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>회원탈퇴</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/member/outForm.jsp</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>회원탈퇴처리</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>회원조회</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/member/selectForm.jsp</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>로그아웃</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/member/joinForm.do</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/member/join.do</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/admin/memberList.do</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/member/modifyForm.do</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/member/modify.do</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/member/outForm.do</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/member/out.do</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/member/select.do</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/member/loginForm.do</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/member/logout.do</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MemberSVCImpl</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>//로그인</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>memberLogin</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>id,pw</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>int (성공여부)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MemberDTO</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/member/modifyForm.jsp</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>/member/loginForm.jsp</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>로그인처리</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>id,pw</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>화면이동</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>회원수정</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/member/modifyForm.jsp</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>회원수정처리</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>회원탈퇴</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/member/outForm.jsp</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>회원탈퇴처리</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>회원조회</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/member/selectForm.jsp</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>로그아웃</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/member/joinForm.do</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/member/join.do</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/admin/memberList.do</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/member/modifyForm.do</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/member/modify.do</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/member/outForm.do</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/member/out.do</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/member/select.do</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/member/loginForm.do</t>
+    <t>MemberSVCImpl</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>/member/login.do</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/member/logout.do</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>MemberSVCImpl</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>//로그인</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>memberLogin</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>id,pw</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>int (성공여부)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>MemberDTO</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -321,7 +325,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -383,13 +387,28 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -421,6 +440,12 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -695,7 +720,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -705,7 +730,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
@@ -742,7 +767,7 @@
         <v>14</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -803,16 +828,16 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="10" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B7" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="D7" s="10" t="s">
         <v>61</v>
-      </c>
-      <c r="C7" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="D7" s="10" t="s">
-        <v>64</v>
       </c>
     </row>
   </sheetData>
@@ -826,8 +851,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A12"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -836,8 +861,8 @@
     <col min="2" max="2" width="24.125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.625" customWidth="1"/>
     <col min="5" max="5" width="21" customWidth="1"/>
-    <col min="6" max="6" width="13.25" customWidth="1"/>
-    <col min="7" max="7" width="15" customWidth="1"/>
+    <col min="6" max="6" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.25" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="19.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -864,7 +889,7 @@
         <v>25</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
@@ -872,7 +897,7 @@
         <v>20</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2" t="s">
@@ -890,7 +915,7 @@
         <v>28</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C3" s="7" t="s">
         <v>14</v>
@@ -900,61 +925,61 @@
       </c>
       <c r="E3" s="7"/>
       <c r="F3" s="7" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="G3" s="7" t="s">
         <v>30</v>
       </c>
       <c r="H3" s="8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="C4" s="11"/>
+      <c r="D4" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="F4" s="11" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6" t="s">
+      <c r="G4" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="H4" s="11"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="E4" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="F4" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="G4" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="H4" s="6"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
+      <c r="E5" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6"/>
     </row>
     <row r="6" spans="1:8" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="8" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C6" s="7" t="s">
         <v>16</v>
@@ -964,7 +989,7 @@
       </c>
       <c r="E6" s="7"/>
       <c r="F6" s="7" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="G6" s="7" t="s">
         <v>30</v>
@@ -975,17 +1000,17 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="9" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C7" s="6"/>
       <c r="D7" s="9" t="s">
         <v>26</v>
       </c>
       <c r="E7" s="9" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F7" s="6"/>
       <c r="G7" s="6"/>
@@ -993,10 +1018,10 @@
     </row>
     <row r="8" spans="1:8" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="8" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C8" s="7" t="s">
         <v>16</v>
@@ -1006,7 +1031,7 @@
       </c>
       <c r="E8" s="7"/>
       <c r="F8" s="7" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="G8" s="7" t="s">
         <v>30</v>
@@ -1015,64 +1040,64 @@
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A9" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="B9" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="C9" s="6" t="s">
+    <row r="9" spans="1:8" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="B9" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="C9" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="D9" s="9" t="s">
+      <c r="D9" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="E9" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="F9" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="G9" s="6" t="s">
+      <c r="E9" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="F9" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="G9" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="H9" s="6"/>
+      <c r="H9" s="11"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A10" s="4" t="s">
+      <c r="A10" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="B10" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="C10" s="2"/>
-      <c r="D10" s="4" t="s">
+      <c r="B10" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="C10" s="6"/>
+      <c r="D10" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="E10" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
+      <c r="E10" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>36</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>37</v>
       </c>
       <c r="D11" s="4" t="s">
         <v>29</v>
       </c>
       <c r="E11" s="2"/>
       <c r="F11" s="2" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="G11" s="2" t="s">
         <v>30</v>
@@ -1083,10 +1108,10 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C12" s="4" t="s">
         <v>16</v>

</xml_diff>

<commit_message>
doc: 2020-01-16 공부한 내용 저장
</commit_message>
<xml_diff>
--- a/documents/20200114/회원관리URL매핑정책.xlsx
+++ b/documents/20200114/회원관리URL매핑정책.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="82">
   <si>
     <t>기능</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -278,6 +278,70 @@
   </si>
   <si>
     <t>/member/login.do</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>아이디찾기(화면)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/member/findID.do</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GET</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>아이디찾기(Restful)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/member/id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">/member/findID.jsp </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MemberSVCImpl</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MemberDAOImpl</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>비밀번호찾기(화면)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/member/findPW.do</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">/member/findPW.jsp </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MemberSVCImpl</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>id.tel,birth</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>tel,birth</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/member/pw</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>비밀번호찾기(Restful)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -720,7 +784,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -849,10 +913,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H12"/>
+  <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1126,6 +1190,86 @@
         <v>32</v>
       </c>
     </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="C13" s="2"/>
+      <c r="D13" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A14" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="H14" s="2"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A15" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="C15" s="2"/>
+      <c r="D15" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A16" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="H16" s="2"/>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
doc: 2020-01-17 공부한 내용 추가
</commit_message>
<xml_diff>
--- a/documents/20200114/회원관리URL매핑정책.xlsx
+++ b/documents/20200114/회원관리URL매핑정책.xlsx
@@ -209,139 +209,139 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>/member/modifyForm.do</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/member/modify.do</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/member/outForm.do</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/member/out.do</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/member/select.do</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/member/loginForm.do</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/member/logout.do</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MemberSVCImpl</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>//로그인</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>memberLogin</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>id,pw</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>int (성공여부)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MemberDTO</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/member/modifyForm.jsp</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/member/loginForm.jsp</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MemberSVCImpl</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/member/login.do</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>아이디찾기(화면)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/member/findID.do</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GET</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>아이디찾기(Restful)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/member/id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">/member/findID.jsp </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MemberSVCImpl</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MemberDAOImpl</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>비밀번호찾기(화면)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/member/findPW.do</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">/member/findPW.jsp </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MemberSVCImpl</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>id.tel,birth</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>tel,birth</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/member/pw</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>비밀번호찾기(Restful)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>/admin/memberList.do</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/member/modifyForm.do</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/member/modify.do</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/member/outForm.do</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/member/out.do</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/member/select.do</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/member/loginForm.do</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/member/logout.do</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>MemberSVCImpl</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>//로그인</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>memberLogin</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>id,pw</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>int (성공여부)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>MemberDTO</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/member/modifyForm.jsp</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/member/loginForm.jsp</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>MemberSVCImpl</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/member/login.do</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>아이디찾기(화면)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/member/findID.do</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>GET</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>아이디찾기(Restful)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/member/id</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">/member/findID.jsp </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>MemberSVCImpl</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>MemberDAOImpl</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>비밀번호찾기(화면)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/member/findPW.do</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">/member/findPW.jsp </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>MemberSVCImpl</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>id.tel,birth</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>tel,birth</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/member/pw</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>비밀번호찾기(Restful)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -784,7 +784,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -831,7 +831,7 @@
         <v>14</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -892,16 +892,16 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="B7" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="B7" s="10" t="s">
+      <c r="C7" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="C7" s="10" t="s">
-        <v>59</v>
-      </c>
       <c r="D7" s="10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -916,7 +916,7 @@
   <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -989,13 +989,13 @@
       </c>
       <c r="E3" s="7"/>
       <c r="F3" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G3" s="7" t="s">
         <v>30</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
@@ -1003,7 +1003,7 @@
         <v>31</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>48</v>
+        <v>81</v>
       </c>
       <c r="C4" s="11"/>
       <c r="D4" s="11" t="s">
@@ -1013,7 +1013,7 @@
         <v>33</v>
       </c>
       <c r="F4" s="11" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G4" s="11" t="s">
         <v>30</v>
@@ -1025,14 +1025,14 @@
         <v>38</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C5" s="6"/>
       <c r="D5" s="6" t="s">
         <v>26</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F5" s="6"/>
       <c r="G5" s="6"/>
@@ -1043,7 +1043,7 @@
         <v>39</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C6" s="7" t="s">
         <v>16</v>
@@ -1053,7 +1053,7 @@
       </c>
       <c r="E6" s="7"/>
       <c r="F6" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G6" s="7" t="s">
         <v>30</v>
@@ -1067,7 +1067,7 @@
         <v>40</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C7" s="6"/>
       <c r="D7" s="9" t="s">
@@ -1085,7 +1085,7 @@
         <v>42</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C8" s="7" t="s">
         <v>16</v>
@@ -1095,7 +1095,7 @@
       </c>
       <c r="E8" s="7"/>
       <c r="F8" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G8" s="7" t="s">
         <v>30</v>
@@ -1109,7 +1109,7 @@
         <v>43</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C9" s="11" t="s">
         <v>16</v>
@@ -1121,7 +1121,7 @@
         <v>44</v>
       </c>
       <c r="F9" s="11" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G9" s="11" t="s">
         <v>30</v>
@@ -1133,14 +1133,14 @@
         <v>34</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C10" s="6"/>
       <c r="D10" s="9" t="s">
         <v>26</v>
       </c>
       <c r="E10" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F10" s="6"/>
       <c r="G10" s="6"/>
@@ -1151,7 +1151,7 @@
         <v>35</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>36</v>
@@ -1161,7 +1161,7 @@
       </c>
       <c r="E11" s="2"/>
       <c r="F11" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G11" s="2" t="s">
         <v>30</v>
@@ -1175,7 +1175,7 @@
         <v>45</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C12" s="4" t="s">
         <v>16</v>
@@ -1192,17 +1192,17 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="B13" s="4" t="s">
         <v>66</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>67</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
@@ -1210,39 +1210,39 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="B14" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="B14" s="4" t="s">
-        <v>70</v>
-      </c>
       <c r="C14" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E14" s="2"/>
       <c r="F14" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="G14" s="2" t="s">
         <v>72</v>
-      </c>
-      <c r="G14" s="2" t="s">
-        <v>73</v>
       </c>
       <c r="H14" s="2"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="B15" s="4" t="s">
         <v>74</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>75</v>
       </c>
       <c r="C15" s="2"/>
       <c r="D15" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
@@ -1250,23 +1250,23 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E16" s="2"/>
       <c r="F16" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H16" s="2"/>
     </row>

</xml_diff>